<commit_message>
Wykresy - nowe dane
</commit_message>
<xml_diff>
--- a/ea3/sprawko elektro.xlsx
+++ b/ea3/sprawko elektro.xlsx
@@ -252,7 +252,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -391,11 +391,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="5387973"/>
-        <c:axId val="9027320"/>
+        <c:axId val="95418523"/>
+        <c:axId val="64668521"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5387973"/>
+        <c:axId val="95418523"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,11 +412,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="9027320"/>
+        <c:crossAx val="64668521"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9027320"/>
+        <c:axId val="64668521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +433,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5387973"/>
+        <c:crossAx val="95418523"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -459,7 +459,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -587,11 +587,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69337414"/>
-        <c:axId val="43582932"/>
+        <c:axId val="29855498"/>
+        <c:axId val="52328808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69337414"/>
+        <c:axId val="29855498"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,11 +608,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="43582932"/>
+        <c:crossAx val="52328808"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43582932"/>
+        <c:axId val="52328808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +629,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69337414"/>
+        <c:crossAx val="29855498"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -655,7 +655,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -886,11 +886,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="8658405"/>
-        <c:axId val="77339649"/>
+        <c:axId val="97255027"/>
+        <c:axId val="42984284"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8658405"/>
+        <c:axId val="97255027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,11 +907,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77339649"/>
+        <c:crossAx val="42984284"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77339649"/>
+        <c:axId val="42984284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,7 +928,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8658405"/>
+        <c:crossAx val="97255027"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -954,7 +954,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1108,11 +1108,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="24512488"/>
-        <c:axId val="48112978"/>
+        <c:axId val="5662073"/>
+        <c:axId val="52118248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="24512488"/>
+        <c:axId val="5662073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,11 +1129,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48112978"/>
+        <c:crossAx val="52118248"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48112978"/>
+        <c:axId val="52118248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,7 +1150,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24512488"/>
+        <c:crossAx val="5662073"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1176,7 +1176,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1292,11 +1292,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="13912170"/>
-        <c:axId val="76897861"/>
+        <c:axId val="7019478"/>
+        <c:axId val="99861642"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13912170"/>
+        <c:axId val="7019478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,11 +1313,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76897861"/>
+        <c:crossAx val="99861642"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76897861"/>
+        <c:axId val="99861642"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1334,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13912170"/>
+        <c:crossAx val="7019478"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1360,7 +1360,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1476,11 +1476,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="14650650"/>
-        <c:axId val="23219082"/>
+        <c:axId val="39509873"/>
+        <c:axId val="65497476"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14650650"/>
+        <c:axId val="39509873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,11 +1497,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23219082"/>
+        <c:crossAx val="65497476"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23219082"/>
+        <c:axId val="65497476"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1518,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14650650"/>
+        <c:crossAx val="39509873"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1544,7 +1544,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1660,11 +1660,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="22592988"/>
-        <c:axId val="86265109"/>
+        <c:axId val="3801361"/>
+        <c:axId val="97414199"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22592988"/>
+        <c:axId val="3801361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,11 +1681,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86265109"/>
+        <c:crossAx val="97414199"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86265109"/>
+        <c:axId val="97414199"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1702,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22592988"/>
+        <c:crossAx val="3801361"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1728,7 +1728,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2075,11 +2075,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="39852663"/>
-        <c:axId val="47234844"/>
+        <c:axId val="27041148"/>
+        <c:axId val="25655127"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39852663"/>
+        <c:axId val="27041148"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,11 +2095,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47234844"/>
+        <c:crossAx val="25655127"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47234844"/>
+        <c:axId val="25655127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2124,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39852663"/>
+        <c:crossAx val="27041148"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2159,7 +2159,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2506,11 +2506,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="99081708"/>
-        <c:axId val="5242004"/>
+        <c:axId val="40997131"/>
+        <c:axId val="88215905"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99081708"/>
+        <c:axId val="40997131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2526,11 +2526,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5242004"/>
+        <c:crossAx val="88215905"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5242004"/>
+        <c:axId val="88215905"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30"/>
@@ -2556,8 +2556,397 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99081708"/>
+        <c:crossAx val="40997131"/>
         <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprawność w funkcji mocy oddanej</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>wypr</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wypr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$4:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>52.9084</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.4666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.935</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.4764</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.3174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.585</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$L$4:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>61.5213953488372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0289130434783</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.0357142857143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.3362264150943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.219298245614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.9814754098361</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.7576923076923</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.0367647058824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>przem</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>przem</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$16:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.9366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.1814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.8696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.2836</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.1804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$L$16:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>60.6111111111111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.7302631578947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.92075</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.4407317073171</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.8409756097561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.8916853932584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.6597802197802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tyr</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tyr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$28:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.6544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.2166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.6904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.6776</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.9796</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.6656</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$L$28:$L$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>55.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.4634375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.778125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.2929230769231</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.9963636363636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.1224615384615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.2859375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="2994777"/>
+        <c:axId val="18025971"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2994777"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="18025971"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="18025971"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2994777"/>
+        <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2863,6 +3252,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>341280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>677880</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11517120" y="4112280"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2873,8 +3292,8 @@
   </sheetPr>
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>